<commit_message>
destek hesaplaması-destek alan kişi 1 olursa transpose t() değişitirildi.
</commit_message>
<xml_diff>
--- a/data/dosya_bilgiler.xlsx
+++ b/data/dosya_bilgiler.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gokhan.usta\Desktop\ProInsure\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F5487D-B472-4BF3-BED6-35E5E6C84D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71045FE-14FE-458F-BC9A-92C60EBC1F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29970" yWindow="1170" windowWidth="25035" windowHeight="11535" activeTab="1" xr2:uid="{FDCA984E-B360-4523-ACB0-EAF1AAE9C561}"/>
+    <workbookView xWindow="900" yWindow="2475" windowWidth="26760" windowHeight="12420" activeTab="1" xr2:uid="{FDCA984E-B360-4523-ACB0-EAF1AAE9C561}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="50">
   <si>
     <t>Cinsiyet</t>
   </si>
@@ -184,22 +184,10 @@
     <t>Yok</t>
   </si>
   <si>
-    <t>Nimet AYRIÇAL</t>
-  </si>
-  <si>
-    <t>Bekir AYRIÇAL</t>
-  </si>
-  <si>
-    <t>Tuğba AYRIÇAL</t>
-  </si>
-  <si>
-    <t>Hava DUVAR</t>
-  </si>
-  <si>
-    <t>Rahim DUVAR</t>
-  </si>
-  <si>
-    <t>s</t>
+    <t>test</t>
+  </si>
+  <si>
+    <t>testtest</t>
   </si>
 </sst>
 </file>
@@ -705,10 +693,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7E1469-5423-4871-A537-FD77751D4660}">
-  <dimension ref="A1:AA11"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,10 +799,10 @@
         <v>16</v>
       </c>
       <c r="D2" s="7">
-        <v>27519</v>
+        <v>15862</v>
       </c>
       <c r="E2" s="7">
-        <v>45037</v>
+        <v>45357</v>
       </c>
       <c r="F2" t="s">
         <v>42</v>
@@ -823,16 +811,16 @@
         <v>49</v>
       </c>
       <c r="H2" s="7">
-        <v>24067</v>
+        <v>23530</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="K2" s="7">
-        <v>37798</v>
+        <v>45502</v>
       </c>
       <c r="L2" t="s">
         <v>45</v>
@@ -859,33 +847,28 @@
         <v>45502</v>
       </c>
       <c r="T2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="U2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="V2" s="7">
-        <v>19382</v>
+        <v>45502</v>
       </c>
       <c r="W2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="X2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="Y2" s="7">
-        <v>18936</v>
+        <v>45502</v>
       </c>
       <c r="Z2">
         <v>100</v>
       </c>
       <c r="AA2">
         <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="W11" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>